<commit_message>
Memory added. Data deleted by error
</commit_message>
<xml_diff>
--- a/Assigment 2/MATRICES.xlsx
+++ b/Assigment 2/MATRICES.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javix\Documents\2ºUni\PADSOFT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\2º Universidad\Segundo Cuatrimestre\PADSOFT\Practicas\Assigment 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1" xr2:uid="{1792376B-6A5D-45ED-BA8D-3966E1136770}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="50">
   <si>
     <t>FR1-Search by ZIP, date and offer type</t>
   </si>
@@ -165,13 +165,22 @@
     <t>removeCharacteristic</t>
   </si>
   <si>
-    <t>FR13-See alL the made offers</t>
+    <t>searchLoggedIn</t>
+  </si>
+  <si>
+    <t>sumDebtMoney</t>
+  </si>
+  <si>
+    <t>isValid</t>
+  </si>
+  <si>
+    <t>FR13-See all the made offers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -209,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -323,19 +332,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -343,17 +339,6 @@
       <bottom style="thick">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -623,6 +608,73 @@
       </top>
       <bottom style="thick">
         <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -630,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -647,83 +699,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1037,7 +1095,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE58D22-26B7-4A72-8076-25F5104F0894}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1051,11 +1109,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353BFF08-0AE3-42B4-9128-F3BC0FF9DA90}">
-  <dimension ref="C4:AF25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,157 +1130,173 @@
     <col min="12" max="12" width="15.28515625" customWidth="1"/>
     <col min="13" max="13" width="16.5703125" customWidth="1"/>
     <col min="14" max="14" width="22.7109375" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1"/>
-    <col min="17" max="17" width="35.140625" customWidth="1"/>
-    <col min="18" max="18" width="18.85546875" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" customWidth="1"/>
-    <col min="21" max="21" width="12.5703125" customWidth="1"/>
-    <col min="22" max="22" width="11.140625" customWidth="1"/>
-    <col min="23" max="23" width="15.140625" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" customWidth="1"/>
-    <col min="25" max="25" width="16.28515625" customWidth="1"/>
-    <col min="26" max="26" width="14.5703125" customWidth="1"/>
-    <col min="27" max="27" width="11.140625" customWidth="1"/>
-    <col min="28" max="28" width="16.5703125" customWidth="1"/>
-    <col min="29" max="29" width="15.7109375" customWidth="1"/>
-    <col min="30" max="30" width="18.28515625" customWidth="1"/>
-    <col min="31" max="31" width="18.42578125" customWidth="1"/>
-    <col min="32" max="32" width="22" customWidth="1"/>
+    <col min="15" max="16" width="20.7109375" customWidth="1"/>
+    <col min="18" max="18" width="38.140625" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" customWidth="1"/>
+    <col min="24" max="24" width="16.7109375" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" customWidth="1"/>
+    <col min="27" max="27" width="16.28515625" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" customWidth="1"/>
+    <col min="29" max="29" width="11.140625" customWidth="1"/>
+    <col min="30" max="30" width="16.5703125" customWidth="1"/>
+    <col min="31" max="31" width="15.7109375" customWidth="1"/>
+    <col min="32" max="33" width="18.28515625" customWidth="1"/>
+    <col min="34" max="34" width="18.42578125" customWidth="1"/>
+    <col min="35" max="35" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="3:32" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="20"/>
-      <c r="D5" s="15" t="s">
+    <row r="4" spans="3:35" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+    </row>
+    <row r="5" spans="3:35" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="17"/>
+      <c r="D5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="M5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="N5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="28" t="s">
+      <c r="P5" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" s="31"/>
+      <c r="S5" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="S5" s="26" t="s">
+      <c r="T5" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="T5" s="26" t="s">
+      <c r="U5" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="U5" s="26" t="s">
+      <c r="V5" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="V5" s="26" t="s">
+      <c r="W5" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="W5" s="26" t="s">
+      <c r="X5" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y5" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="X5" s="26" t="s">
+      <c r="Z5" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="26" t="s">
+      <c r="AA5" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="Z5" s="26" t="s">
+      <c r="AB5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="AA5" s="26" t="s">
+      <c r="AC5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="AB5" s="26" t="s">
+      <c r="AD5" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AC5" s="26" t="s">
+      <c r="AE5" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AD5" s="26" t="s">
+      <c r="AF5" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="AE5" s="26" t="s">
+      <c r="AG5" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH5" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="AF5" s="27" t="s">
+      <c r="AI5" s="24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="3:32" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="21" t="s">
+    <row r="6" spans="3:35" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="12"/>
-      <c r="Q6" s="33" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="39"/>
+      <c r="R6" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="R6" s="29"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="25"/>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="25"/>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="25"/>
-      <c r="AD6" s="25"/>
-      <c r="AE6" s="25"/>
-      <c r="AF6" s="35"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22"/>
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="22"/>
+      <c r="AH6" s="22"/>
+      <c r="AI6" s="32"/>
     </row>
-    <row r="7" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="22" t="s">
+    <row r="7" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="14" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="5"/>
@@ -1235,15 +1309,15 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
-      <c r="O7" s="6"/>
-      <c r="Q7" s="31" t="s">
+      <c r="O7" s="2"/>
+      <c r="P7" s="40"/>
+      <c r="R7" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="R7" s="4"/>
-      <c r="S7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T7" s="2"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
@@ -1255,34 +1329,39 @@
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
-      <c r="AF7" s="36"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="33"/>
     </row>
-    <row r="8" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="23" t="s">
+    <row r="8" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="8"/>
-      <c r="Q8" s="30" t="s">
+      <c r="D8" s="15"/>
+      <c r="E8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="R8" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="R8" s="3"/>
-      <c r="S8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="T8" s="1"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
@@ -1294,13 +1373,16 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
-      <c r="AF8" s="37"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="34"/>
     </row>
-    <row r="9" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="22" t="s">
+    <row r="9" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="17"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -1311,70 +1393,82 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="6"/>
-      <c r="Q9" s="31" t="s">
+      <c r="O9" s="2"/>
+      <c r="P9" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="R9" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="R9" s="4"/>
-      <c r="S9" s="2"/>
+      <c r="S9" s="4"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
-      <c r="Z9" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
+      <c r="AB9" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
-      <c r="AF9" s="36"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="33"/>
     </row>
-    <row r="10" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="23" t="s">
+    <row r="10" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="8"/>
-      <c r="Q10" s="30" t="s">
+      <c r="D10" s="15"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="R10" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R10" s="3"/>
-      <c r="S10" s="1"/>
+      <c r="S10" s="3"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
+      <c r="X10" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
-      <c r="AA10" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
+      <c r="AC10" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="AD10" s="1"/>
       <c r="AE10" s="1"/>
-      <c r="AF10" s="37"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="34"/>
     </row>
-    <row r="11" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="22" t="s">
+    <row r="11" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="17"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -1387,12 +1481,12 @@
         <v>31</v>
       </c>
       <c r="N11" s="5"/>
-      <c r="O11" s="6"/>
-      <c r="Q11" s="31" t="s">
+      <c r="O11" s="2"/>
+      <c r="P11" s="40"/>
+      <c r="R11" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="R11" s="4"/>
-      <c r="S11" s="2"/>
+      <c r="S11" s="4"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
@@ -1401,39 +1495,44 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
-      <c r="AB11" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
-      <c r="AD11" s="2"/>
+      <c r="AD11" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="AE11" s="2"/>
-      <c r="AF11" s="36"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="33"/>
     </row>
-    <row r="12" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="23" t="s">
+    <row r="12" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q12" s="30" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P12" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="R12" s="3"/>
-      <c r="S12" s="1"/>
+      <c r="S12" s="3"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
@@ -1446,13 +1545,16 @@
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
-      <c r="AF12" s="37"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="34"/>
     </row>
-    <row r="13" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="22" t="s">
+    <row r="13" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="17"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -1463,12 +1565,14 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
-      <c r="O13" s="6"/>
-      <c r="Q13" s="31" t="s">
+      <c r="O13" s="2"/>
+      <c r="P13" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="R13" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="R13" s="4"/>
-      <c r="S13" s="2"/>
+      <c r="S13" s="4"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
@@ -1478,41 +1582,46 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
-      <c r="AC13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE13" s="2"/>
-      <c r="AF13" s="36"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="33"/>
     </row>
-    <row r="14" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="23" t="s">
+    <row r="14" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="8"/>
-      <c r="Q14" s="30" t="s">
+      <c r="D14" s="15"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="R14" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="R14" s="3"/>
-      <c r="S14" s="1"/>
+      <c r="S14" s="3"/>
       <c r="T14" s="1"/>
-      <c r="U14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="V14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
@@ -1522,13 +1631,16 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
       <c r="AE14" s="1"/>
-      <c r="AF14" s="37"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="34"/>
     </row>
-    <row r="15" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="22" t="s">
+    <row r="15" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="17"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1541,18 +1653,20 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
-      <c r="O15" s="6"/>
-      <c r="Q15" s="31" t="s">
+      <c r="O15" s="2"/>
+      <c r="P15" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="R15" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="R15" s="4"/>
-      <c r="S15" s="2"/>
+      <c r="S15" s="4"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
-      <c r="V15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="W15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
@@ -1561,31 +1675,38 @@
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
       <c r="AE15" s="2"/>
-      <c r="AF15" s="36"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="33"/>
     </row>
-    <row r="16" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="23" t="s">
+    <row r="16" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="8"/>
-      <c r="Q16" s="30" t="s">
+      <c r="D16" s="15"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="R16" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="R16" s="3"/>
-      <c r="S16" s="1"/>
+      <c r="S16" s="3"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
@@ -1598,13 +1719,16 @@
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
-      <c r="AF16" s="37"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="34"/>
     </row>
-    <row r="17" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="22" t="s">
+    <row r="17" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="17"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1615,12 +1739,14 @@
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
-      <c r="O17" s="6"/>
-      <c r="Q17" s="31" t="s">
+      <c r="O17" s="2"/>
+      <c r="P17" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="R17" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="R17" s="4"/>
-      <c r="S17" s="2"/>
+      <c r="S17" s="4"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
@@ -1632,40 +1758,45 @@
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
-      <c r="AE17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF17" s="36" t="s">
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI17" s="33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="23" t="s">
+    <row r="18" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="8"/>
-      <c r="Q18" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="R18" s="3"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U18" s="1"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="R18" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="S18" s="3"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
@@ -1676,13 +1807,16 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
       <c r="AE18" s="1"/>
-      <c r="AF18" s="37"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="34"/>
     </row>
-    <row r="19" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="22" t="s">
+    <row r="19" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="17"/>
+      <c r="D19" s="14"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1693,12 +1827,14 @@
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="6"/>
-      <c r="Q19" s="31" t="s">
+      <c r="O19" s="2"/>
+      <c r="P19" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="R19" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="R19" s="4"/>
-      <c r="S19" s="2"/>
+      <c r="S19" s="4"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
@@ -1710,41 +1846,48 @@
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
-      <c r="AE19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF19" s="36"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI19" s="33"/>
     </row>
-    <row r="20" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="23" t="s">
+    <row r="20" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="8"/>
-      <c r="Q20" s="30" t="s">
+      <c r="D20" s="15"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="R20" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="R20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="T20" s="1"/>
+      <c r="S20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
+      <c r="X20" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
@@ -1752,13 +1895,16 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
-      <c r="AF20" s="37"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="34"/>
     </row>
-    <row r="21" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="22" t="s">
+    <row r="21" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="17"/>
+      <c r="D21" s="14"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -1769,70 +1915,82 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
-      <c r="O21" s="6"/>
-      <c r="Q21" s="31" t="s">
+      <c r="O21" s="2"/>
+      <c r="P21" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="R21" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="R21" s="4"/>
-      <c r="S21" s="2"/>
+      <c r="S21" s="4"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
-      <c r="W21" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="W21" s="2"/>
       <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
+      <c r="Y21" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
       <c r="AE21" s="2"/>
-      <c r="AF21" s="36"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="33"/>
     </row>
-    <row r="22" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="23" t="s">
+    <row r="22" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="8"/>
-      <c r="Q22" s="30" t="s">
+      <c r="D22" s="15"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="R22" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="R22" s="3"/>
-      <c r="S22" s="1"/>
+      <c r="S22" s="3"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
-      <c r="Y22" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
+      <c r="AA22" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
       <c r="AE22" s="1"/>
-      <c r="AF22" s="37"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="34"/>
     </row>
-    <row r="23" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="22" t="s">
+    <row r="23" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="17"/>
+      <c r="D23" s="14"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -1843,68 +2001,78 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
-      <c r="O23" s="6"/>
-      <c r="Q23" s="31" t="s">
+      <c r="O23" s="2"/>
+      <c r="P23" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="R23" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="R23" s="4"/>
-      <c r="S23" s="2"/>
+      <c r="S23" s="4"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
-      <c r="X23" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
-      <c r="Z23" s="2"/>
+      <c r="Z23" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
       <c r="AE23" s="2"/>
-      <c r="AF23" s="36"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="33"/>
     </row>
-    <row r="24" spans="3:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="24" t="s">
+    <row r="24" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="10"/>
-      <c r="Q24" s="32" t="s">
+      <c r="D24" s="16"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R24" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="R24" s="38"/>
-      <c r="S24" s="39"/>
-      <c r="T24" s="39"/>
-      <c r="U24" s="39"/>
-      <c r="V24" s="39"/>
-      <c r="W24" s="39"/>
-      <c r="X24" s="39"/>
-      <c r="Y24" s="39"/>
-      <c r="Z24" s="39"/>
-      <c r="AA24" s="39"/>
-      <c r="AB24" s="39"/>
-      <c r="AC24" s="39"/>
-      <c r="AD24" s="39"/>
-      <c r="AE24" s="39"/>
-      <c r="AF24" s="40"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="36"/>
+      <c r="U24" s="36"/>
+      <c r="V24" s="36"/>
+      <c r="W24" s="36"/>
+      <c r="X24" s="36"/>
+      <c r="Y24" s="36"/>
+      <c r="Z24" s="36"/>
+      <c r="AA24" s="36"/>
+      <c r="AB24" s="36"/>
+      <c r="AC24" s="36"/>
+      <c r="AD24" s="36"/>
+      <c r="AE24" s="36"/>
+      <c r="AF24" s="36"/>
+      <c r="AG24" s="36"/>
+      <c r="AH24" s="36"/>
+      <c r="AI24" s="37"/>
     </row>
-    <row r="25" spans="3:32" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="3:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>